<commit_message>
DWH-11: Fix MasterData tests
</commit_message>
<xml_diff>
--- a/importer/src/test/resources/zipcode_locations.xlsx
+++ b/importer/src/test/resources/zipcode_locations.xlsx
@@ -152,13 +152,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C59"/>
+  <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.0078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.17"/>
@@ -190,7 +190,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>456465</v>
+        <v>456466</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>47.4564697894</v>
@@ -199,9 +199,18 @@
         <v>19.45467878754</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="1"/>
-    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="1"/>
+    </row>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>